<commit_message>
show hide collapsed btn
</commit_message>
<xml_diff>
--- a/WebAppChat.xlsx
+++ b/WebAppChat.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\chatApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F9D2079-A1E7-44E4-A66F-D1CB69153A39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C3A5ED-4BD1-4C32-B1C0-ACA386CE2A12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7455" yWindow="1950" windowWidth="18495" windowHeight="12510" activeTab="1" xr2:uid="{6456D250-3D17-463E-985F-D203F4A2C4A6}"/>
+    <workbookView xWindow="8820" yWindow="1470" windowWidth="18495" windowHeight="12510" activeTab="1" xr2:uid="{6456D250-3D17-463E-985F-D203F4A2C4A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -444,15 +444,7 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>content: &lt;userID&gt;</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>title object</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>uint64</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
@@ -476,10 +468,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>ID: &lt;titleID&gt;</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>type: &lt;like/unlike&gt;</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -491,12 +479,24 @@
     <t>likes: &lt;user list&gt;</t>
     <phoneticPr fontId="2"/>
   </si>
+  <si>
+    <t>zID</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>content: &lt;user.zID&gt;</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>zID: &lt;title.zID&gt;</t>
+    <phoneticPr fontId="2"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -537,6 +537,15 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="163"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -717,7 +726,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -788,6 +797,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -6103,6 +6121,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8974198-09F5-4A4B-B3AB-D2807BA22D2E}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Q79"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
@@ -6871,10 +6890,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C145D31D-6BF1-4306-92E9-72F0C25D4F4E}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:P37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="M34" sqref="M34"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -6889,7 +6909,7 @@
         <v>40</v>
       </c>
       <c r="M2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.4">
@@ -6897,10 +6917,10 @@
         <v>41</v>
       </c>
       <c r="M3" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="N3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.4">
@@ -6911,7 +6931,7 @@
         <v>9</v>
       </c>
       <c r="N4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.4">
@@ -6919,7 +6939,7 @@
         <v>38</v>
       </c>
       <c r="N5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.4">
@@ -6930,7 +6950,7 @@
         <v>19</v>
       </c>
       <c r="N6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.4">
@@ -6941,21 +6961,21 @@
         <v>16</v>
       </c>
       <c r="N7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.4">
       <c r="E8" t="s">
         <v>45</v>
       </c>
-      <c r="M8" t="s">
-        <v>64</v>
-      </c>
-      <c r="N8" t="s">
+      <c r="M8" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="N8" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="O8" s="26" t="s">
         <v>63</v>
-      </c>
-      <c r="O8" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.4">
@@ -6968,7 +6988,7 @@
         <v>47</v>
       </c>
       <c r="M10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.4">
@@ -6999,7 +7019,7 @@
       <c r="H14" s="2"/>
       <c r="I14" s="3"/>
       <c r="M14" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.4">
@@ -7092,7 +7112,7 @@
         <v>54</v>
       </c>
       <c r="M20" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="P20" t="s">
         <v>51</v>
@@ -7169,10 +7189,10 @@
         <v>52</v>
       </c>
       <c r="M26" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="P26" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.4">
@@ -7185,7 +7205,7 @@
       <c r="H27" s="5"/>
       <c r="I27" s="6"/>
       <c r="M27" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.4">
@@ -7198,7 +7218,7 @@
       <c r="H28" s="5"/>
       <c r="I28" s="6"/>
       <c r="M28" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.4">
@@ -7250,7 +7270,7 @@
         <v>54</v>
       </c>
       <c r="M32" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="P32" t="s">
         <v>51</v>
@@ -7266,7 +7286,7 @@
       <c r="H33" s="5"/>
       <c r="I33" s="6"/>
       <c r="M33" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.4">
@@ -7279,7 +7299,7 @@
       <c r="H34" s="5"/>
       <c r="I34" s="6"/>
       <c r="M34" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.4">
@@ -7304,13 +7324,13 @@
       <c r="G36" s="8"/>
       <c r="H36" s="8"/>
       <c r="I36" s="9"/>
-      <c r="M36" s="16" t="s">
-        <v>70</v>
+      <c r="M36" s="25" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.4">
-      <c r="M37" s="16" t="s">
-        <v>71</v>
+      <c r="M37" s="24" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -7323,6 +7343,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E48B14B7-59B7-48A8-B8DC-EECE67438311}">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>